<commit_message>
Adding new G. raimondii unclustered verification to table
</commit_message>
<xml_diff>
--- a/manuscript/first_draft/T4b_CNVrecovered.xlsx
+++ b/manuscript/first_draft/T4b_CNVrecovered.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Projects\Kokia\SourceTree\manuscript\first_draft\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9300"/>
+    <workbookView xWindow="51200" yWindow="2700" windowWidth="33600" windowHeight="21000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>by clustering</t>
   </si>
@@ -93,12 +91,30 @@
   </si>
   <si>
     <t>514 (35%)</t>
+  </si>
+  <si>
+    <t>G. kirkii unclustered verification</t>
+  </si>
+  <si>
+    <t>K. drynarioides unclustered verification</t>
+  </si>
+  <si>
+    <t>"good" translations</t>
+  </si>
+  <si>
+    <t>overlapping annotations</t>
+  </si>
+  <si>
+    <t>valid and overlapping</t>
+  </si>
+  <si>
+    <t>G. raimondii unclustered genes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -136,6 +152,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -196,7 +213,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -231,7 +248,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -408,7 +425,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -416,24 +433,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="38.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="38.33203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +461,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -458,7 +475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -469,7 +486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -483,7 +500,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -494,7 +511,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +519,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -512,16 +529,18 @@
       <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -532,7 +551,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -540,8 +559,70 @@
         <v>22</v>
       </c>
     </row>
+    <row r="18" spans="1:6">
+      <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="1">
+        <v>10408</v>
+      </c>
+      <c r="C19" s="1">
+        <v>6229</v>
+      </c>
+      <c r="D19" s="1">
+        <v>3330</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1983</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1">
+        <v>10408</v>
+      </c>
+      <c r="C20" s="1">
+        <v>6035</v>
+      </c>
+      <c r="D20" s="1">
+        <v>3513</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2009</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1527</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>